<commit_message>
more function and prompt
</commit_message>
<xml_diff>
--- a/single.xlsx
+++ b/single.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350BD655-2AFD-4F22-BA1D-85ECD282A202}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2971340E-07AF-4BA8-9D7F-F316635D72A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>型號 / Model name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,22 @@
   </si>
   <si>
     <t>分類</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出處</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>衝突</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -376,55 +392,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="52.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>